<commit_message>
added support for new indexes
</commit_message>
<xml_diff>
--- a/Market Exposure_COPY.xlsx
+++ b/Market Exposure_COPY.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="766" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="766" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="7" r:id="rId1"/>
@@ -31,6 +31,208 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Tony Stark</author>
+  </authors>
+  <commentList>
+    <comment ref="A21" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+S&amp;P Toronto 60</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A22" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Amsterdam Exchange Index.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A23" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+OMX Stockholm 30</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A24" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+MDAX</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Swiss Market Index</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+FTSE JSE top 40</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+OBX Index</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A29" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Tony Stark:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+TecDAX</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Tony Stark</author>
@@ -2321,7 +2523,7 @@
 </comments>
 </file>
 
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Tony Stark</author>
@@ -2956,7 +3158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="448">
   <si>
     <t>Name</t>
   </si>
@@ -4287,6 +4489,33 @@
   <si>
     <t>TP/SL%</t>
   </si>
+  <si>
+    <t>CA60</t>
+  </si>
+  <si>
+    <t>NETH25</t>
+  </si>
+  <si>
+    <t>SE30</t>
+  </si>
+  <si>
+    <t>MidDE60</t>
+  </si>
+  <si>
+    <t>SWI20</t>
+  </si>
+  <si>
+    <t>CHINAH</t>
+  </si>
+  <si>
+    <t>SA40</t>
+  </si>
+  <si>
+    <t>NOR25</t>
+  </si>
+  <si>
+    <t>TecDE30</t>
+  </si>
 </sst>
 </file>
 
@@ -4845,7 +5074,37 @@
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
     <cellStyle name="Warning Text" xfId="3" builtinId="11"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="16">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5296,7 +5555,7 @@
         <v>408</v>
       </c>
       <c r="E4" s="16">
-        <f>SUM(Commodity!E20,Index!E24,ETF!D34,Bonds!E14,FOREX!C30,Stocks!D121)</f>
+        <f>SUM(Commodity!E20,Index!E33,ETF!D34,Bonds!E14,FOREX!C30,Stocks!D121)</f>
         <v>0</v>
       </c>
     </row>
@@ -5306,7 +5565,7 @@
         <v>409</v>
       </c>
       <c r="E5" s="81">
-        <f>SUM(Commodity!F20,Index!F24,Stocks!E121,ETF!E34,Bonds!F14,FOREX!C31)</f>
+        <f>SUM(Commodity!F20,Index!F33,Stocks!E121,ETF!E34,Bonds!F14,FOREX!C31)</f>
         <v>0</v>
       </c>
       <c r="F5" s="46"/>
@@ -5429,7 +5688,7 @@
         <v>425</v>
       </c>
       <c r="E14" s="11">
-        <f>Index!E24</f>
+        <f>Index!E33</f>
         <v>0</v>
       </c>
       <c r="F14" s="42"/>
@@ -5550,7 +5809,7 @@
         <v>425</v>
       </c>
       <c r="E22" s="125">
-        <f>Index!F24</f>
+        <f>Index!F33</f>
         <v>0</v>
       </c>
       <c r="F22" s="42"/>
@@ -5830,7 +6089,7 @@
     <mergeCell ref="D3:E3"/>
   </mergeCells>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="greaterThan">
       <formula>20</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6496,11 +6755,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:N33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6509,7 +6768,7 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.28515625" customWidth="1"/>
     <col min="7" max="7" width="10" style="25" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
@@ -6626,42 +6885,42 @@
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="91">
-        <f>Live!B7</f>
-        <v>1.2608299999999999</v>
+        <f>$C$6</f>
+        <v>1.0975200000000001</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="88">
-        <f t="shared" ref="E7:E23" si="0">(B7*C7)*D7</f>
+        <f t="shared" ref="E7:E26" si="0">(B7*C7)*D7</f>
         <v>0</v>
       </c>
       <c r="F7" s="96">
-        <f t="shared" ref="F7:F23" si="1">E7/$B$2</f>
+        <f t="shared" ref="F7:F29" si="1">E7/$B$2</f>
         <v>0</v>
       </c>
       <c r="G7" s="54"/>
       <c r="H7" s="63">
-        <f t="shared" ref="H7:H20" si="2">F7*G7</f>
+        <f t="shared" ref="H7:H29" si="2">F7*G7</f>
         <v>0</v>
       </c>
       <c r="I7" s="38">
-        <f t="shared" ref="I7:I23" si="3">H7*$B$2</f>
+        <f t="shared" ref="I7:I29" si="3">H7*$B$2</f>
         <v>0</v>
       </c>
       <c r="J7" s="18"/>
       <c r="K7" s="63">
-        <f t="shared" ref="K7:K20" si="4">J7*F7</f>
+        <f t="shared" ref="K7:K29" si="4">J7*F7</f>
         <v>0</v>
       </c>
       <c r="L7" s="38">
-        <f t="shared" ref="L7:L23" si="5">K7*$B$2</f>
+        <f t="shared" ref="L7:L29" si="5">K7*$B$2</f>
         <v>0</v>
       </c>
       <c r="M7" s="122">
-        <f t="shared" ref="M7:M20" si="6">(B7*G7)+B7</f>
+        <f t="shared" ref="M7:M29" si="6">(B7*G7)+B7</f>
         <v>0</v>
       </c>
       <c r="N7" s="123">
-        <f t="shared" ref="N7:N20" si="7">B7-(B7*K7)</f>
+        <f t="shared" ref="N7:N29" si="7">B7-(B7*K7)</f>
         <v>0</v>
       </c>
     </row>
@@ -6671,8 +6930,8 @@
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="91">
-        <f>Live!B8</f>
-        <v>0.64039000000000001</v>
+        <f>$C$6</f>
+        <v>1.0975200000000001</v>
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="88">
@@ -6993,7 +7252,7 @@
       </c>
       <c r="B16" s="7"/>
       <c r="C16" s="91">
-        <f>C6</f>
+        <f>$C$6</f>
         <v>1.0975200000000001</v>
       </c>
       <c r="D16" s="6"/>
@@ -7171,7 +7430,7 @@
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="91">
-        <f>C6</f>
+        <f>$C$6</f>
         <v>1.0975200000000001</v>
       </c>
       <c r="D20" s="6"/>
@@ -7211,17 +7470,58 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="F21" s="99"/>
-      <c r="G21" s="14"/>
-      <c r="N21" s="12"/>
+      <c r="A21" s="86" t="s">
+        <v>439</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="91">
+        <f>Live!$B$13</f>
+        <v>1.39035</v>
+      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="88">
+        <f>(B21/C21)*D21</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G21" s="6"/>
+      <c r="H21" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I21" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J21" s="6"/>
+      <c r="K21" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L21" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M21" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N21" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="86" t="s">
-        <v>105</v>
+        <v>440</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="86">
-        <v>1</v>
+      <c r="C22" s="91">
+        <f>$C$6</f>
+        <v>1.0975200000000001</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="88">
@@ -7232,9 +7532,9 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G22" s="54"/>
+      <c r="G22" s="101"/>
       <c r="H22" s="63">
-        <f t="shared" ref="H22" si="8">F22*G22</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I22" s="38">
@@ -7243,7 +7543,7 @@
       </c>
       <c r="J22" s="6"/>
       <c r="K22" s="63">
-        <f t="shared" ref="K22" si="9">J22*F22</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L22" s="38">
@@ -7251,34 +7551,35 @@
         <v>0</v>
       </c>
       <c r="M22" s="122">
-        <f t="shared" ref="M22" si="10">(B22*G22)+B22</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N22" s="123">
-        <f t="shared" ref="N22" si="11">B22-(B22*K22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="86" t="s">
-        <v>106</v>
+        <v>441</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="86">
-        <v>1</v>
-      </c>
-      <c r="D23" s="67"/>
+      <c r="C23" s="91">
+        <f>Live!$B$16</f>
+        <v>9.9605200000000007</v>
+      </c>
+      <c r="D23" s="6"/>
       <c r="E23" s="88">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F23" s="97">
+        <f>(B23/C23)*D23</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="96">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G23" s="54"/>
+      <c r="G23" s="101"/>
       <c r="H23" s="63">
-        <f t="shared" ref="H23" si="12">F23*G23</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I23" s="38">
@@ -7287,7 +7588,7 @@
       </c>
       <c r="J23" s="6"/>
       <c r="K23" s="63">
-        <f t="shared" ref="K23" si="13">J23*F23</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L23" s="38">
@@ -7295,83 +7596,447 @@
         <v>0</v>
       </c>
       <c r="M23" s="122">
-        <f t="shared" ref="M23" si="14">(B23*G23)+B23</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N23" s="123">
-        <f t="shared" ref="N23" si="15">B23-(B23*K23)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D24" s="59" t="s">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="86" t="s">
+        <v>442</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="91">
+        <f>$C$6</f>
+        <v>1.0975200000000001</v>
+      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F24" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="101"/>
+      <c r="H24" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="6"/>
+      <c r="K24" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M24" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N24" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="86" t="s">
+        <v>443</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="91">
+        <f>Live!$B$12</f>
+        <v>0.96109999999999995</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="88">
+        <f>(B25/C25)*D25</f>
+        <v>0</v>
+      </c>
+      <c r="F25" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="101"/>
+      <c r="H25" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="6"/>
+      <c r="K25" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M25" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N25" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="86" t="s">
+        <v>444</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="91">
+        <f>$C$18</f>
+        <v>0.12900695605507048</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="88">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F26" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="101"/>
+      <c r="H26" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="6"/>
+      <c r="K26" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M26" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N26" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="86" t="s">
+        <v>445</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="91">
+        <f>Live!$B$18</f>
+        <v>18.338339999999999</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="88">
+        <f>(B27/C27)*D27</f>
+        <v>0</v>
+      </c>
+      <c r="F27" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="101"/>
+      <c r="H27" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="6"/>
+      <c r="K27" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L27" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M27" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N27" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="86" t="s">
+        <v>446</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="91">
+        <f>Live!$B$15</f>
+        <v>10.320819999999999</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="88">
+        <f>(B28/C28)*D28</f>
+        <v>0</v>
+      </c>
+      <c r="F28" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="101"/>
+      <c r="H28" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I28" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J28" s="6"/>
+      <c r="K28" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L28" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M28" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N28" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="86" t="s">
+        <v>447</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="91">
+        <f>$C$6</f>
+        <v>1.0975200000000001</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="88">
+        <f t="shared" ref="E29" si="8">(B29*C29)*D29</f>
+        <v>0</v>
+      </c>
+      <c r="F29" s="96">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="101"/>
+      <c r="H29" s="63">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="38">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="6"/>
+      <c r="K29" s="63">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="38">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="122">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="123">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="86" t="s">
+        <v>105</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="86">
+        <v>1</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="88">
+        <f>(B31*C31)*D31</f>
+        <v>0</v>
+      </c>
+      <c r="F31" s="96">
+        <f>E31/$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="G31" s="54"/>
+      <c r="H31" s="63">
+        <f t="shared" ref="H31" si="9">F31*G31</f>
+        <v>0</v>
+      </c>
+      <c r="I31" s="38">
+        <f>H31*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="J31" s="6"/>
+      <c r="K31" s="63">
+        <f t="shared" ref="K31" si="10">J31*F31</f>
+        <v>0</v>
+      </c>
+      <c r="L31" s="38">
+        <f>K31*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="M31" s="122">
+        <f t="shared" ref="M31" si="11">(B31*G31)+B31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="123">
+        <f t="shared" ref="N31" si="12">B31-(B31*K31)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="86" t="s">
+        <v>106</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="86">
+        <v>1</v>
+      </c>
+      <c r="D32" s="67"/>
+      <c r="E32" s="88">
+        <f>(B32*C32)*D32</f>
+        <v>0</v>
+      </c>
+      <c r="F32" s="97">
+        <f>E32/$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="G32" s="54"/>
+      <c r="H32" s="63">
+        <f t="shared" ref="H32" si="13">F32*G32</f>
+        <v>0</v>
+      </c>
+      <c r="I32" s="38">
+        <f>H32*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="J32" s="6"/>
+      <c r="K32" s="63">
+        <f t="shared" ref="K32" si="14">J32*F32</f>
+        <v>0</v>
+      </c>
+      <c r="L32" s="38">
+        <f>K32*$B$2</f>
+        <v>0</v>
+      </c>
+      <c r="M32" s="122">
+        <f t="shared" ref="M32" si="15">(B32*G32)+B32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="123">
+        <f t="shared" ref="N32" si="16">B32-(B32*K32)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D33" s="59" t="s">
         <v>410</v>
       </c>
-      <c r="E24" s="85">
-        <f>SUM(E6:E23)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="98">
-        <f>SUM(F6:F23)</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="77">
-        <f>SUM(H6:H23)</f>
-        <v>0</v>
-      </c>
-      <c r="I24" s="70">
-        <f>SUM(I6:I23)</f>
-        <v>0</v>
-      </c>
-      <c r="J24" s="14"/>
-      <c r="K24" s="77">
-        <f>SUM(K6:K23)</f>
-        <v>0</v>
-      </c>
-      <c r="L24" s="127">
-        <f>SUM(L6:L23)</f>
-        <v>0</v>
-      </c>
-      <c r="M24" s="14"/>
-      <c r="N24" s="14"/>
+      <c r="E33" s="85">
+        <f>SUM(E6:E32)</f>
+        <v>0</v>
+      </c>
+      <c r="F33" s="98">
+        <f>SUM(F6:F32)</f>
+        <v>0</v>
+      </c>
+      <c r="G33" s="14"/>
+      <c r="H33" s="77">
+        <f>SUM(H6:H32)</f>
+        <v>0</v>
+      </c>
+      <c r="I33" s="70">
+        <f>SUM(I6:I32)</f>
+        <v>0</v>
+      </c>
+      <c r="J33" s="14"/>
+      <c r="K33" s="77">
+        <f>SUM(K6:K32)</f>
+        <v>0</v>
+      </c>
+      <c r="L33" s="127">
+        <f>SUM(L6:L32)</f>
+        <v>0</v>
+      </c>
+      <c r="M33" s="14"/>
+      <c r="N33" s="14"/>
     </row>
   </sheetData>
   <sortState ref="A12:H12">
     <sortCondition ref="A11"/>
   </sortState>
-  <conditionalFormatting sqref="F6:F14 F16:F20 F22:F23">
-    <cfRule type="cellIs" dxfId="11" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="F6:F14 F16:F20 F31:F32">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="10" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="F33">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H24">
-    <cfRule type="cellIs" dxfId="9" priority="4" operator="greaterThan">
+  <conditionalFormatting sqref="H33">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I24">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+  <conditionalFormatting sqref="I33">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K24">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="K33">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
       <formula>10</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L24">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="L33">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
       <formula>10</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21:F29">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13013,27 +13678,27 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E8:E68">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="7" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E70:E120">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E121">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G121">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J121">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
       <formula>5</formula>
     </cfRule>
   </conditionalFormatting>
@@ -60421,7 +61086,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:F13">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="greaterThan">
       <formula>2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -60435,7 +61100,7 @@
   <dimension ref="A2:AI162"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="AG10" sqref="AG10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65905,8 +66570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>